<commit_message>
finalizacao dos testes nao parametricos
</commit_message>
<xml_diff>
--- a/R/elsa/dados_elsa/Lucia_Andrade_variáveis.xlsx
+++ b/R/elsa/dados_elsa/Lucia_Andrade_variáveis.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Lucia_Andrade_variáveis_CSV" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Lucia_Andrade_variáveis_CSV" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2490,6 +2490,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2497,15 +2603,15 @@
   </sheetPr>
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B202" activeCellId="0" sqref="B202"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="79.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.64"/>
   </cols>
@@ -2545,7 +2651,7 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -2562,7 +2668,7 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -2579,7 +2685,7 @@
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="1" t="n">

</xml_diff>

<commit_message>
ajustes estatisticos do elsa
</commit_message>
<xml_diff>
--- a/R/elsa/dados_elsa/Lucia_Andrade_variáveis.xlsx
+++ b/R/elsa/dados_elsa/Lucia_Andrade_variáveis.xlsx
@@ -2603,8 +2603,8 @@
   </sheetPr>
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B383" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C403" activeCellId="0" sqref="C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>